<commit_message>
fix updates for class
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="742" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="742"/>
   </bookViews>
   <sheets>
     <sheet name="announcements" sheetId="7" r:id="rId1"/>
@@ -432,9 +432,6 @@
     <t xml:space="preserve">You can see the course schedule [here](schedule.html) and syllabus [here](syllabus.html). </t>
   </si>
   <si>
-    <t>We will not have class next week due to the Annual AFS meeting in Tampa.</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -790,6 +787,9 @@
   </si>
   <si>
     <t>No class: university holiday</t>
+  </si>
+  <si>
+    <t>We will not have class on 8/22 due to the Annual AFS meeting in Atlantic City</t>
   </si>
 </sst>
 </file>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>106</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1288,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1300,7 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+    <sheetView topLeftCell="C10" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -1405,7 +1405,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>51</v>
@@ -1440,7 +1440,7 @@
         <v>43348</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>22</v>
@@ -1712,7 +1712,7 @@
         <v>36</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>37</v>
@@ -1750,7 +1750,7 @@
         <v>38</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>41</v>
@@ -1788,7 +1788,7 @@
         <v>45</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>42</v>
@@ -1826,7 +1826,7 @@
         <v>43</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>53</v>
@@ -1943,7 +1943,7 @@
         <v>30</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2012,7 +2012,7 @@
         <v>60</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>59</v>
@@ -2035,10 +2035,10 @@
         <v>43339</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2069,7 +2069,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
       <c r="E4" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2082,7 +2082,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2100,7 +2100,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2113,7 +2113,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2126,7 +2126,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2157,7 +2157,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
       <c r="E10" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2170,7 +2170,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
       <c r="E11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2188,7 +2188,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" s="24"/>
     </row>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2887,13 +2887,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="11" t="s">
         <v>132</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="D18" s="11"/>
       <c r="F18" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2923,10 +2923,10 @@
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="D20" s="11"/>
       <c r="F20" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H20" s="11"/>
     </row>
@@ -2959,7 +2959,7 @@
         <v>94</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2989,7 +2989,7 @@
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3033,13 +3033,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>94</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -3053,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3067,10 +3067,10 @@
         <v>0</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -3114,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3128,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="23"/>
@@ -3144,13 +3144,13 @@
         <v>0</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>94</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3179,10 +3179,10 @@
         <v>0</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3196,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3210,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3224,13 +3224,13 @@
         <v>0</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3246,7 +3246,7 @@
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3264,7 +3264,7 @@
         <v>94</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3279,10 +3279,10 @@
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3298,7 +3298,7 @@
       <c r="D42" s="22"/>
       <c r="E42" s="10"/>
       <c r="F42" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="20" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3314,7 +3314,7 @@
       <c r="D43" s="22"/>
       <c r="E43" s="10"/>
       <c r="F43" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F44" s="23"/>
     </row>
@@ -3344,13 +3344,13 @@
         <v>0</v>
       </c>
       <c r="D45" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F45" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3364,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3379,10 +3379,10 @@
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3400,7 +3400,7 @@
         <v>94</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="D49" s="22"/>
       <c r="F49" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -3430,7 +3430,7 @@
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -3444,10 +3444,10 @@
         <v>0</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3461,13 +3461,13 @@
         <v>0</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -3481,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -3495,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -3509,10 +3509,10 @@
         <v>0</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -3526,10 +3526,10 @@
         <v>0</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -3543,10 +3543,10 @@
         <v>0</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3560,10 +3560,10 @@
         <v>0</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3577,10 +3577,10 @@
         <v>0</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -3594,10 +3594,10 @@
         <v>0</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -3611,10 +3611,10 @@
         <v>0</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -3628,10 +3628,10 @@
         <v>0</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -3645,10 +3645,10 @@
         <v>0</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -3662,7 +3662,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -3676,10 +3676,10 @@
         <v>0</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -3693,10 +3693,10 @@
         <v>0</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -3710,10 +3710,10 @@
         <v>0</v>
       </c>
       <c r="D67" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>208</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -3727,10 +3727,10 @@
         <v>0</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -3744,10 +3744,10 @@
         <v>0</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -3761,10 +3761,10 @@
         <v>0</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -3778,10 +3778,10 @@
         <v>0</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -3828,10 +3828,10 @@
         <v>61</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>62</v>
@@ -3839,13 +3839,13 @@
     </row>
     <row r="2" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="D2" s="11" t="str">
         <f t="shared" ref="D2:D11" si="0">CONCATENATE(B2," [pdf](pdfs/",C2,")")</f>
@@ -3854,13 +3854,13 @@
     </row>
     <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>113</v>
       </c>
       <c r="D3" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3869,13 +3869,13 @@
     </row>
     <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="D4" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3884,13 +3884,13 @@
     </row>
     <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="D5" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3899,13 +3899,13 @@
     </row>
     <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>98</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3914,13 +3914,13 @@
     </row>
     <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>99</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3929,13 +3929,13 @@
     </row>
     <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="D8" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3944,10 +3944,10 @@
     </row>
     <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="str">
@@ -3957,13 +3957,13 @@
     </row>
     <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>125</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>126</v>
       </c>
       <c r="D10" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3972,13 +3972,13 @@
     </row>
     <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="D11" s="11" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
class deck up date
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="742"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="742" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="announcements" sheetId="7" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="223">
   <si>
     <t>Week</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Invasive species II</t>
   </si>
   <si>
-    <t>Commercial fisheries management I</t>
-  </si>
-  <si>
     <t>Commercial fisheries management II</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
   </si>
   <si>
     <t>Recreation fisheries management II</t>
-  </si>
-  <si>
-    <t>Conservation Fisheries</t>
   </si>
   <si>
     <t>_Exam I_</t>
@@ -1243,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,13 +1249,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1269,10 +1263,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -1280,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1288,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1300,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1364,7 @@
         <v>10</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1402,13 +1396,13 @@
         <v>43341</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -1440,13 +1434,13 @@
         <v>43348</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
         <v>23</v>
@@ -1481,13 +1475,13 @@
         <v>43355</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1522,7 +1516,7 @@
         <v>25</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>26</v>
@@ -1557,10 +1551,10 @@
         <v>43369</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>27</v>
@@ -1598,7 +1592,7 @@
         <v>28</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>32</v>
@@ -1636,7 +1630,7 @@
         <v>29</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>33</v>
@@ -1674,7 +1668,7 @@
         <v>34</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>35</v>
@@ -1712,10 +1706,10 @@
         <v>36</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>37</v>
+        <v>218</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1724,7 +1718,7 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" si="4"/>
-        <v>29 October: Commercial fisheries management I</v>
+        <v>29 October: Recreation fisheries management I</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -1732,7 +1726,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="2"/>
-        <v>31 October: Commercial fisheries management II</v>
+        <v>31 October: Recreation fisheries management II</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="3"/>
@@ -1746,23 +1740,23 @@
         <f t="shared" si="1"/>
         <v>43404</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>38</v>
+      <c r="H12" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="4"/>
-        <v>5 November: Recreation fisheries management I</v>
+        <v>5 November: Commercial fisheries management II</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -1770,7 +1764,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="2"/>
-        <v>7 November: _Exam II_</v>
+        <v>7 November: Commercial fisheries management II</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="3"/>
@@ -1784,14 +1778,14 @@
         <f t="shared" si="1"/>
         <v>43411</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>45</v>
+      <c r="H13" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>42</v>
+        <v>217</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1800,7 +1794,7 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="4"/>
-        <v>12 November: Recreation fisheries management II</v>
+        <v>12 November: Commercial fisheries management II</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -1808,7 +1802,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="2"/>
-        <v>14 November: Conservation Fisheries</v>
+        <v>14 November: Evolution and management</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" si="3"/>
@@ -1822,15 +1816,16 @@
         <f t="shared" si="1"/>
         <v>43418</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1838,7 +1833,7 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="4"/>
-        <v>19 November: Evolution and management</v>
+        <v>19 November: _Exam II_</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -1861,7 +1856,7 @@
         <v>43425</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>31</v>
@@ -1899,13 +1894,13 @@
         <v>43432</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="J16" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1937,13 +1932,13 @@
         <v>43439</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1974,7 +1969,7 @@
         <v>12</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J18" s="5"/>
     </row>
@@ -2009,19 +2004,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2035,10 +2030,10 @@
         <v>43339</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2056,7 +2051,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2069,7 +2064,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
       <c r="E4" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2082,7 +2077,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2100,7 +2095,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2113,7 +2108,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="13"/>
       <c r="E7" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2126,7 +2121,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2141,10 +2136,10 @@
         <v>43360</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2157,7 +2152,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="13"/>
       <c r="E10" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2170,7 +2165,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
       <c r="E11" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2185,10 +2180,10 @@
         <v>43367</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F12" s="24"/>
     </row>
@@ -2204,10 +2199,10 @@
         <v>43374</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2222,10 +2217,10 @@
         <v>43381</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2238,7 +2233,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
       <c r="E15" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2251,7 +2246,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
       <c r="E16" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2264,7 +2259,7 @@
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
       <c r="E17" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2277,7 +2272,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
       <c r="E18" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2292,10 +2287,10 @@
         <v>43388</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2308,7 +2303,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
       <c r="E20" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2321,7 +2316,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="13"/>
       <c r="E21" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2334,7 +2329,7 @@
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
       <c r="E22" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -2347,7 +2342,7 @@
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2362,10 +2357,10 @@
         <v>43395</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2378,7 +2373,7 @@
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
       <c r="E25" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -2391,7 +2386,7 @@
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
       <c r="E26" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2406,10 +2401,10 @@
         <v>43402</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -2422,7 +2417,7 @@
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
       <c r="E28" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2435,7 +2430,7 @@
       <c r="C29" s="12"/>
       <c r="D29" s="13"/>
       <c r="E29" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -2448,7 +2443,7 @@
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
       <c r="E30" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2463,10 +2458,10 @@
         <v>43409</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -2479,7 +2474,7 @@
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
       <c r="E32" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2490,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -2501,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2516,10 +2511,10 @@
         <v>43416</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2532,7 +2527,7 @@
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
       <c r="E36" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -2545,7 +2540,7 @@
       <c r="C37" s="12"/>
       <c r="D37" s="13"/>
       <c r="E37" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -2563,7 +2558,7 @@
         <v>31</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2578,10 +2573,10 @@
         <v>43430</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -2596,10 +2591,10 @@
         <v>43437</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -2630,22 +2625,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="F1" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2659,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2673,13 +2668,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2694,7 +2689,7 @@
       </c>
       <c r="D4" s="11"/>
       <c r="F4" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2709,7 +2704,7 @@
       </c>
       <c r="D5" s="11"/>
       <c r="F5" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2724,7 +2719,7 @@
       </c>
       <c r="D6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2739,7 +2734,7 @@
       </c>
       <c r="D7" s="11"/>
       <c r="F7" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2753,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2767,10 +2762,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -2785,7 +2780,7 @@
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="72.599999999999994" x14ac:dyDescent="0.3">
@@ -2800,7 +2795,7 @@
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
@@ -2815,7 +2810,7 @@
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24.6" x14ac:dyDescent="0.3">
@@ -2830,7 +2825,7 @@
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="60.6" x14ac:dyDescent="0.3">
@@ -2845,7 +2840,7 @@
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -2859,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2873,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2887,13 +2882,13 @@
         <v>0</v>
       </c>
       <c r="D17" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2908,7 +2903,7 @@
       </c>
       <c r="D18" s="11"/>
       <c r="F18" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2923,10 +2918,10 @@
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2941,7 +2936,7 @@
       </c>
       <c r="D20" s="11"/>
       <c r="F20" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H20" s="11"/>
     </row>
@@ -2956,10 +2951,10 @@
         <v>0</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2974,7 +2969,7 @@
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2989,7 +2984,7 @@
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -3004,7 +2999,7 @@
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -3019,7 +3014,7 @@
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3033,13 +3028,13 @@
         <v>0</v>
       </c>
       <c r="D26" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -3053,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3067,10 +3062,10 @@
         <v>0</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3085,7 +3080,7 @@
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -3100,7 +3095,7 @@
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -3114,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3128,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="23"/>
@@ -3144,13 +3139,13 @@
         <v>0</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -3165,7 +3160,7 @@
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3179,10 +3174,10 @@
         <v>0</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3196,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -3210,7 +3205,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3224,13 +3219,13 @@
         <v>0</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3246,7 +3241,7 @@
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3261,10 +3256,10 @@
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3279,10 +3274,10 @@
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3298,7 +3293,7 @@
       <c r="D42" s="22"/>
       <c r="E42" s="10"/>
       <c r="F42" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="20" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3314,7 +3309,7 @@
       <c r="D43" s="22"/>
       <c r="E43" s="10"/>
       <c r="F43" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -3329,7 +3324,7 @@
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F44" s="23"/>
     </row>
@@ -3344,13 +3339,13 @@
         <v>0</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3364,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3379,10 +3374,10 @@
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3397,10 +3392,10 @@
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -3415,7 +3410,7 @@
       </c>
       <c r="D49" s="22"/>
       <c r="F49" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -3430,7 +3425,7 @@
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -3444,10 +3439,10 @@
         <v>0</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3461,13 +3456,13 @@
         <v>0</v>
       </c>
       <c r="D52" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -3481,7 +3476,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -3495,7 +3490,7 @@
         <v>0</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -3509,10 +3504,10 @@
         <v>0</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -3526,10 +3521,10 @@
         <v>0</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -3543,10 +3538,10 @@
         <v>0</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3560,10 +3555,10 @@
         <v>0</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3577,10 +3572,10 @@
         <v>0</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -3594,10 +3589,10 @@
         <v>0</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -3611,10 +3606,10 @@
         <v>0</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -3628,10 +3623,10 @@
         <v>0</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -3645,10 +3640,10 @@
         <v>0</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -3662,7 +3657,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -3676,10 +3671,10 @@
         <v>0</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -3693,10 +3688,10 @@
         <v>0</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -3710,10 +3705,10 @@
         <v>0</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -3727,10 +3722,10 @@
         <v>0</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -3744,10 +3739,10 @@
         <v>0</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -3761,10 +3756,10 @@
         <v>0</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -3778,10 +3773,10 @@
         <v>0</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -3825,27 +3820,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>110</v>
       </c>
       <c r="D2" s="11" t="str">
         <f t="shared" ref="D2:D11" si="0">CONCATENATE(B2," [pdf](pdfs/",C2,")")</f>
@@ -3854,13 +3849,13 @@
     </row>
     <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3869,13 +3864,13 @@
     </row>
     <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="D4" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3884,13 +3879,13 @@
     </row>
     <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D5" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3899,13 +3894,13 @@
     </row>
     <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3914,13 +3909,13 @@
     </row>
     <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D7" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3929,13 +3924,13 @@
     </row>
     <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>122</v>
       </c>
       <c r="D8" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3944,10 +3939,10 @@
     </row>
     <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11" t="str">
@@ -3957,13 +3952,13 @@
     </row>
     <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3972,13 +3967,13 @@
     </row>
     <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D11" s="11" t="str">
         <f t="shared" si="0"/>

</xml_diff>